<commit_message>
Outputted info to excel sheet (sorted by last name)
</commit_message>
<xml_diff>
--- a/Customer Onboarding Automation/cust_data.xlsx
+++ b/Customer Onboarding Automation/cust_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20370"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brerj\Documents\uni\4.2\762\project\Customer Onboarding Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\762_RPA\INFOSYS300-SE762-Team-1\Customer Onboarding Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3FCDA0E-1679-4D25-BDEB-BF2FE03B55BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCAF30C-E089-45D4-B286-9C8331AEB31A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FA51CD74-A4F3-4AF9-A491-C8F03D3CC86E}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" xr2:uid="{FA51CD74-A4F3-4AF9-A491-C8F03D3CC86E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,19 +20,199 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+  <si>
+    <t>Full name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Contact number</t>
+  </si>
+  <si>
+    <t>Email address</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>David Brown</t>
+  </si>
+  <si>
+    <t>101 Pine Street, Dunedin, NZ</t>
+  </si>
+  <si>
+    <t>021 333 7890</t>
+  </si>
+  <si>
+    <t>david.brown@email.com</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Bob Clark</t>
+  </si>
+  <si>
+    <t>555 Walnut Avenue, Palmerston North, NZ</t>
+  </si>
+  <si>
+    <t>+64 20 444 9876</t>
+  </si>
+  <si>
+    <t>bob.clark@email.com</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>Adam Doe</t>
+  </si>
+  <si>
+    <t>456 Elm Avenue, Wellington, NZ</t>
+  </si>
+  <si>
+    <t>+64 22 987 6543</t>
+  </si>
+  <si>
+    <t>adam_doe@email.com</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>Peter Harris</t>
+  </si>
+  <si>
+    <t>777 Spruce Lane, Invercargill, NZ</t>
+  </si>
+  <si>
+    <t>64 22 555 2345</t>
+  </si>
+  <si>
+    <t>peter.harris@email.co.nz</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Harris</t>
+  </si>
+  <si>
+    <t>Emily Johnson</t>
+  </si>
+  <si>
+    <t>emily.johnson@email.com</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Michael Lee</t>
+  </si>
+  <si>
+    <t>333 Birch Lane, Tauranga, NZ</t>
+  </si>
+  <si>
+    <t>+64 22 111 5678</t>
+  </si>
+  <si>
+    <t>michaellee1@email.com</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Jane Smith</t>
+  </si>
+  <si>
+    <t>123 Main Street, Auckland, NZ</t>
+  </si>
+  <si>
+    <t>jane.smith@email.com</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Lisa Taylor</t>
+  </si>
+  <si>
+    <t>444 Maple Street, Napier, NZ</t>
+  </si>
+  <si>
+    <t>+64 27 888 8765</t>
+  </si>
+  <si>
+    <t>lisa.taylor@email.com</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Karen White</t>
+  </si>
+  <si>
+    <t>666 Redwood Drive, Rotorua, NZ</t>
+  </si>
+  <si>
+    <t>+64 21 222 3456</t>
+  </si>
+  <si>
+    <t>karen.white@email.com</t>
+  </si>
+  <si>
+    <t>Karen</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Zara Wilson</t>
+  </si>
+  <si>
+    <t>789 Oak Drive, Christchurch, NZ</t>
+  </si>
+  <si>
+    <t>zarawilson@email.com</t>
+  </si>
+  <si>
+    <t>Zara</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,12 +562,227 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B65CE4-B689-479C-AF9C-76390711401F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>216784321</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8">
+        <v>64211234567</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
4: Added Validation Details
</commit_message>
<xml_diff>
--- a/Customer Onboarding Automation/cust_data.xlsx
+++ b/Customer Onboarding Automation/cust_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20370"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\762_RPA\INFOSYS300-SE762-Team-1\Customer Onboarding Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Avikash\Documents\UiPath\INFOSYS300-SE762-Team-1\Customer Onboarding Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCAF30C-E089-45D4-B286-9C8331AEB31A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C523C9D-F459-41AD-889E-C6C510658617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" xr2:uid="{FA51CD74-A4F3-4AF9-A491-C8F03D3CC86E}"/>
+    <workbookView xWindow="3930" yWindow="3000" windowWidth="21600" windowHeight="11295" xr2:uid="{FA51CD74-A4F3-4AF9-A491-C8F03D3CC86E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t>Full name</t>
   </si>
@@ -211,16 +211,51 @@
   </si>
   <si>
     <t>Wilson</t>
+  </si>
+  <si>
+    <t>Test User</t>
+  </si>
+  <si>
+    <t>20 Symonds Street, Auckland, NZ</t>
+  </si>
+  <si>
+    <t>test.user@email.com</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>02041166935</t>
+  </si>
+  <si>
+    <t>Test User2</t>
+  </si>
+  <si>
+    <t>21 Symonds Street, Auckland, NZ</t>
+  </si>
+  <si>
+    <t>User2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -243,13 +278,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -562,11 +601,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B65CE4-B689-479C-AF9C-76390711401F}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -782,7 +829,47 @@
         <v>61</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D12" r:id="rId1" xr:uid="{1AA34311-2AEE-43BE-9996-AA673791E2BF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>